<commit_message>
plot accident rate depends on location and year
</commit_message>
<xml_diff>
--- a/accident_data.xlsx
+++ b/accident_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuiwatanabe/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuiwatanabe/Desktop/R/first_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{829B00A7-8051-A245-8795-A9996AE3B874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284750E2-5A9A-8E45-B6D4-058D094A179B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14820" yWindow="500" windowWidth="13600" windowHeight="16420" xr2:uid="{423C42B1-B600-9F4B-A061-1952B517BECF}"/>
+    <workbookView xWindow="14820" yWindow="500" windowWidth="13600" windowHeight="16380" xr2:uid="{423C42B1-B600-9F4B-A061-1952B517BECF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="6">
   <si>
     <t>year</t>
   </si>
@@ -403,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB1C073-790B-1543-AC8E-D228EEEBF487}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -536,6 +536,104 @@
         <v>4</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2016</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2017</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2016</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2017</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2016</v>
+      </c>
+      <c r="B16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2017</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2016</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2017</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2016</v>
+      </c>
+      <c r="B20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2017</v>
+      </c>
+      <c r="B21">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add disengaged by mutate
</commit_message>
<xml_diff>
--- a/accident_data.xlsx
+++ b/accident_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuiwatanabe/Desktop/R/first_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{284750E2-5A9A-8E45-B6D4-058D094A179B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7C3547-D534-3B48-AD99-899DD06D0FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14820" yWindow="500" windowWidth="13600" windowHeight="16380" xr2:uid="{423C42B1-B600-9F4B-A061-1952B517BECF}"/>
   </bookViews>
@@ -406,7 +406,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>